<commit_message>
deep sea double count fix
</commit_message>
<xml_diff>
--- a/output/aggregate_tables/Area Statistics/area_21_summary.xlsx
+++ b/output/aggregate_tables/Area Statistics/area_21_summary.xlsx
@@ -1321,7 +1321,7 @@
         </is>
       </c>
       <c r="C3" s="4" t="n">
-        <v>1.00232117553715</v>
+        <v>0.9823068853471902</v>
       </c>
     </row>
     <row r="4">
@@ -1332,7 +1332,7 @@
         </is>
       </c>
       <c r="C4" s="4" t="n">
-        <v>0.2327224185607216</v>
+        <v>0.2254840312804062</v>
       </c>
     </row>
     <row r="5">
@@ -1343,7 +1343,7 @@
         </is>
       </c>
       <c r="C5" s="4" t="n">
-        <v>1.217294726105878</v>
+        <v>1.197280435915919</v>
       </c>
     </row>
     <row r="6">
@@ -1354,7 +1354,7 @@
         </is>
       </c>
       <c r="C6" s="4" t="n">
-        <v>0.2327224185607216</v>
+        <v>0.2254840312804062</v>
       </c>
     </row>
     <row r="7">
@@ -1369,7 +1369,7 @@
         </is>
       </c>
       <c r="C7" s="4" t="n">
-        <v>14.82558681181366</v>
+        <v>15.10956701022704</v>
       </c>
     </row>
     <row r="8">
@@ -1380,7 +1380,7 @@
         </is>
       </c>
       <c r="C8" s="4" t="n">
-        <v>69.12478098785597</v>
+        <v>69.04212945962217</v>
       </c>
     </row>
     <row r="9">
@@ -1391,7 +1391,7 @@
         </is>
       </c>
       <c r="C9" s="4" t="n">
-        <v>16.04963220033037</v>
+        <v>15.84830353015079</v>
       </c>
     </row>
     <row r="10">
@@ -1402,7 +1402,7 @@
         </is>
       </c>
       <c r="C10" s="4" t="n">
-        <v>83.95036779966964</v>
+        <v>84.15169646984921</v>
       </c>
     </row>
     <row r="11">
@@ -1413,7 +1413,7 @@
         </is>
       </c>
       <c r="C11" s="4" t="n">
-        <v>16.04963220033037</v>
+        <v>15.84830353015079</v>
       </c>
     </row>
   </sheetData>
@@ -1538,31 +1538,31 @@
         <v>0.2149735505687284</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>1.00232117553715</v>
+        <v>0.9823068853471902</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>0.2327224185607216</v>
+        <v>0.2254840312804062</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>1.217294726105878</v>
+        <v>1.197280435915919</v>
       </c>
       <c r="F4" s="4" t="n">
-        <v>0.2327224185607216</v>
+        <v>0.2254840312804062</v>
       </c>
       <c r="G4" s="4" t="n">
-        <v>14.82558681181366</v>
+        <v>15.10956701022704</v>
       </c>
       <c r="H4" s="4" t="n">
-        <v>69.12478098785597</v>
+        <v>69.04212945962217</v>
       </c>
       <c r="I4" s="4" t="n">
-        <v>16.04963220033037</v>
+        <v>15.84830353015079</v>
       </c>
       <c r="J4" s="4" t="n">
-        <v>83.95036779966964</v>
+        <v>84.15169646984921</v>
       </c>
       <c r="K4" s="4" t="n">
-        <v>16.04963220033037</v>
+        <v>15.84830353015079</v>
       </c>
     </row>
     <row r="5">
@@ -1575,31 +1575,31 @@
         <v>0.2149735505687284</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>1.00232117553715</v>
+        <v>0.9823068853471902</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>0.2327224185607216</v>
+        <v>0.2254840312804062</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>1.217294726105878</v>
+        <v>1.197280435915919</v>
       </c>
       <c r="F5" s="4" t="n">
-        <v>0.2327224185607216</v>
+        <v>0.2254840312804062</v>
       </c>
       <c r="G5" s="4" t="n">
-        <v>14.82558681181366</v>
+        <v>15.10956701022704</v>
       </c>
       <c r="H5" s="4" t="n">
-        <v>69.12478098785597</v>
+        <v>69.04212945962217</v>
       </c>
       <c r="I5" s="4" t="n">
-        <v>16.04963220033037</v>
+        <v>15.84830353015079</v>
       </c>
       <c r="J5" s="4" t="n">
-        <v>83.95036779966964</v>
+        <v>84.15169646984921</v>
       </c>
       <c r="K5" s="4" t="n">
-        <v>16.04963220033037</v>
+        <v>15.84830353015079</v>
       </c>
     </row>
     <row r="6">
@@ -1664,7 +1664,7 @@
         </is>
       </c>
       <c r="C2" s="4" t="n">
-        <v>89.62602590419766</v>
+        <v>92.31243281328341</v>
       </c>
     </row>
     <row r="3">
@@ -1675,7 +1675,7 @@
         </is>
       </c>
       <c r="C3" s="4" t="n">
-        <v>14.82558681181366</v>
+        <v>15.10956701022704</v>
       </c>
     </row>
     <row r="4">
@@ -1686,7 +1686,7 @@
         </is>
       </c>
       <c r="C4" s="4" t="n">
-        <v>69.12478098785597</v>
+        <v>69.04212945962217</v>
       </c>
     </row>
     <row r="5">
@@ -1697,7 +1697,7 @@
         </is>
       </c>
       <c r="C5" s="4" t="n">
-        <v>16.04963220033037</v>
+        <v>15.84830353015079</v>
       </c>
     </row>
     <row r="6">
@@ -1708,7 +1708,7 @@
         </is>
       </c>
       <c r="C6" s="4" t="n">
-        <v>83.95036779966964</v>
+        <v>84.15169646984921</v>
       </c>
     </row>
     <row r="7">
@@ -1719,7 +1719,7 @@
         </is>
       </c>
       <c r="C7" s="4" t="n">
-        <v>16.04963220033037</v>
+        <v>15.84830353015079</v>
       </c>
     </row>
     <row r="8">

</xml_diff>